<commit_message>
Team vs Team - 2.0
</commit_message>
<xml_diff>
--- a/Docs/Team_vs_Team.xlsx
+++ b/Docs/Team_vs_Team.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Upwork\ESPN CricInfo Scrape\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3CB5AA-A6C8-4D40-A709-20FF63DAE973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB3168D-7024-4EB1-8F5A-83BD530F8FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,10 +461,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>